<commit_message>
Added solution for task 1.
</commit_message>
<xml_diff>
--- a/Test design/Boundary Value testing/Task_1.xlsx
+++ b/Test design/Boundary Value testing/Task_1.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
+    <sheet name="Solution" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t xml:space="preserve">1 класс: </t>
   </si>
@@ -46,13 +47,52 @@
   </si>
   <si>
     <t>Протестировать программу «Скидка», применяя знания о граничных значениях.</t>
+  </si>
+  <si>
+    <t>Класс</t>
+  </si>
+  <si>
+    <t>Скидка</t>
+  </si>
+  <si>
+    <t>Значение ввода</t>
+  </si>
+  <si>
+    <t>Ожидаемый результат</t>
+  </si>
+  <si>
+    <t>Фактический результат</t>
+  </si>
+  <si>
+    <t>"Введите потраченную сумму"</t>
+  </si>
+  <si>
+    <t>1 класс (0-999)</t>
+  </si>
+  <si>
+    <t>2 класс (1000-4999)</t>
+  </si>
+  <si>
+    <t>3 класс (5000-9999)</t>
+  </si>
+  <si>
+    <t>4 класс (10000&lt;)</t>
+  </si>
+  <si>
+    <t>Статус проверки (+\-)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,8 +107,32 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,8 +145,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEF8F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -105,11 +175,259 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -117,7 +435,73 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -128,6 +512,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFEF8F4"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFE7E7FF"/>
+      <color rgb="FFCCCCFF"/>
       <color rgb="FFE9FFD9"/>
     </mruColors>
   </colors>
@@ -407,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -419,11 +807,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -476,4 +864,271 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <f>B2*C2/100</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="7">
+        <v>500</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D12" si="0">B3*C3/100</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22"/>
+      <c r="B4" s="8">
+        <v>999</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="6">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E5" s="12">
+        <v>50</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="7">
+        <v>2500</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="22"/>
+      <c r="B7" s="8">
+        <v>4999</v>
+      </c>
+      <c r="C7" s="9">
+        <v>5</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>249.95</v>
+      </c>
+      <c r="E7" s="11">
+        <v>249.95</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5000</v>
+      </c>
+      <c r="C8" s="6">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="7">
+        <v>7000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="E9" s="10">
+        <v>700</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="22"/>
+      <c r="B10" s="8">
+        <v>9999</v>
+      </c>
+      <c r="C10" s="9">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>999.9</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10000</v>
+      </c>
+      <c r="C11" s="6">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="E11" s="13">
+        <v>2000</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="8">
+        <v>13000</v>
+      </c>
+      <c r="C12" s="9">
+        <v>15</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>1950</v>
+      </c>
+      <c r="E12" s="15">
+        <v>2600</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>